<commit_message>
added orders/detail models, views, and urls, test ok
</commit_message>
<xml_diff>
--- a/files/project requirements/HU/HU.xlsx
+++ b/files/project requirements/HU/HU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\Administrador\Documents\Documentos personales\MinTIC2022\Ciclo 3\Programación\Proyecto\ssacg\files\project requirements\HU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0172A6-C7EF-48BF-9190-896DF3C1EC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB60D0E2-4AE7-4607-904F-11172543AF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="1" xr2:uid="{DB665A41-5881-4F67-A75C-EB14CE28CF87}"/>
+    <workbookView xWindow="20280" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{DB665A41-5881-4F67-A75C-EB14CE28CF87}"/>
   </bookViews>
   <sheets>
     <sheet name="EPICS" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="259">
   <si>
     <t>ROL</t>
   </si>
@@ -680,6 +680,162 @@
   </si>
   <si>
     <t>1.2.1</t>
+  </si>
+  <si>
+    <t>asginado</t>
+  </si>
+  <si>
+    <t>Construir el modelo de la entidad Cliente</t>
+  </si>
+  <si>
+    <t>Construir el serializador de la entidad Cliente</t>
+  </si>
+  <si>
+    <t>Construir el modelo de la entidad Orden</t>
+  </si>
+  <si>
+    <t>Construir el serializador de la entidad Orden</t>
+  </si>
+  <si>
+    <t>Construir el serializador de la entidad Productos</t>
+  </si>
+  <si>
+    <t>Construir el modelo de la entidad Productos</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Construir el serializador de la entidad detalle de orden</t>
+  </si>
+  <si>
+    <t>Construir el modelo de la entidad detalle de orden</t>
+  </si>
+  <si>
+    <t>Construir el modelo de la entidad Administradores</t>
+  </si>
+  <si>
+    <t>Construir el serializador de la entidad Administradores</t>
+  </si>
+  <si>
+    <t>steven</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>otros (sprint 3)</t>
+  </si>
+  <si>
+    <t>6.1.1</t>
+  </si>
+  <si>
+    <t>Construir un servicio web para autenticar admins</t>
+  </si>
+  <si>
+    <t>6.1.2</t>
+  </si>
+  <si>
+    <t>6.1.3</t>
+  </si>
+  <si>
+    <t>6.1.4</t>
+  </si>
+  <si>
+    <t>6.1.5</t>
+  </si>
+  <si>
+    <t>Diseñar un mockup para autenticar admins (login)</t>
+  </si>
+  <si>
+    <t>Construir UI de mockup para autenticar admins (login)</t>
+  </si>
+  <si>
+    <t>Diseñar casos de prueba para el servicio web de autenticación de admin</t>
+  </si>
+  <si>
+    <t>Realizar casos de prueba para el servicio web de autenticación de admin</t>
+  </si>
+  <si>
+    <t>Diseñar casos de prueba para la UI de autenticación de admins</t>
+  </si>
+  <si>
+    <t>Realizar casos de prueba para la UI de autenticación de admins</t>
+  </si>
+  <si>
+    <t>6.1.6</t>
+  </si>
+  <si>
+    <t>6.1.7</t>
+  </si>
+  <si>
+    <t>6.1.8</t>
+  </si>
+  <si>
+    <t>6.1.9</t>
+  </si>
+  <si>
+    <t>Desplegar servicio web autenticación de admins</t>
+  </si>
+  <si>
+    <t>Desplegar UI autenticación de admins</t>
+  </si>
+  <si>
+    <t>6.6 (registro de admin) parte de 1.2</t>
+  </si>
+  <si>
+    <t>6.6.1</t>
+  </si>
+  <si>
+    <t>6.6.2</t>
+  </si>
+  <si>
+    <t>6.6.3</t>
+  </si>
+  <si>
+    <t>6.6.4</t>
+  </si>
+  <si>
+    <t>6.6.5</t>
+  </si>
+  <si>
+    <t>6.6.6</t>
+  </si>
+  <si>
+    <t>6.6.7</t>
+  </si>
+  <si>
+    <t>6.6.8</t>
+  </si>
+  <si>
+    <t>6.6.9</t>
+  </si>
+  <si>
+    <t>Construir un servicio web para registrar admins</t>
+  </si>
+  <si>
+    <t>Diseñar un mockup para registrar admins</t>
+  </si>
+  <si>
+    <t>Construir UI de mockup para registrar admins</t>
+  </si>
+  <si>
+    <t>Diseñar casos de prueba para el servicio web de registro de admin</t>
+  </si>
+  <si>
+    <t>Realizar casos de prueba para el servicio web de registro de admin</t>
+  </si>
+  <si>
+    <t>Diseñar casos de prueba para la UI de registro de admins</t>
+  </si>
+  <si>
+    <t>Realizar casos de prueba para la UI de registro de admins</t>
+  </si>
+  <si>
+    <t>Desplegar servicio web registro de admins</t>
+  </si>
+  <si>
+    <t>Desplegar UI registro de admins</t>
   </si>
 </sst>
 </file>
@@ -731,7 +887,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -786,8 +942,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -835,12 +997,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -936,6 +1107,28 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -978,18 +1171,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1006,6 +1187,18 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1042,26 +1235,20 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0E140770-7765-4347-8890-6B4C94FC0DD6}" name="HU" displayName="HU" ref="A1:I33" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:I33" xr:uid="{0E140770-7765-4347-8890-6B4C94FC0DD6}">
-    <filterColumn colId="5">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I33" xr:uid="{0E140770-7765-4347-8890-6B4C94FC0DD6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I33">
     <sortCondition ref="B1:B33"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{28171A87-EC5E-4F00-B431-156702AEACD1}" name="ID" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{3D57EC37-28F4-4400-A574-E0E4A54C828A}" name="MÓDULO" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{7DCC34B7-548D-47A7-87E0-7C2F6DAB3DEE}" name="ROL" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{F6FCAAF3-62B9-4B8B-B52A-81D2AC9613FF}" name="FUNCIONALIDAD" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{0AC39ECF-CF32-4750-879E-7F9D09B6DDB4}" name="OBJETIVO" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{C4950150-4523-42DB-B797-688C0BAA5C1F}" name="TAG 1" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{28051DBA-1FB2-4D73-81C0-D9F45456246C}" name="CATEGORÍA" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{28171A87-EC5E-4F00-B431-156702AEACD1}" name="ID" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{3D57EC37-28F4-4400-A574-E0E4A54C828A}" name="MÓDULO" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{7DCC34B7-548D-47A7-87E0-7C2F6DAB3DEE}" name="ROL" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{F6FCAAF3-62B9-4B8B-B52A-81D2AC9613FF}" name="FUNCIONALIDAD" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{0AC39ECF-CF32-4750-879E-7F9D09B6DDB4}" name="OBJETIVO" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{C4950150-4523-42DB-B797-688C0BAA5C1F}" name="TAG 1" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{28051DBA-1FB2-4D73-81C0-D9F45456246C}" name="CATEGORÍA" dataDxfId="6"/>
     <tableColumn id="10" xr3:uid="{AC15AB67-0459-4A71-951D-05D3188B5095}" name="WIREFRAMES"/>
-    <tableColumn id="11" xr3:uid="{268C71AF-9866-41C1-BED0-22AB5BF07941}" name="MOCKUPS" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{268C71AF-9866-41C1-BED0-22AB5BF07941}" name="MOCKUPS" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1367,7 +1554,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA2B2BC-3E42-4558-A732-C5D74C5B836E}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1733,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1.3</v>
       </c>
@@ -1614,7 +1801,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2.2999999999999998</v>
       </c>
@@ -1682,7 +1869,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>3.3</v>
       </c>
@@ -1702,7 +1889,7 @@
       <c r="G10" s="6"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>3.4</v>
       </c>
@@ -1726,7 +1913,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>3.5</v>
       </c>
@@ -1746,7 +1933,7 @@
       <c r="G12" s="6"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>3.6</v>
       </c>
@@ -1766,7 +1953,7 @@
       <c r="G13" s="6"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>3.7</v>
       </c>
@@ -1786,7 +1973,7 @@
       <c r="G14" s="6"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>3.8</v>
       </c>
@@ -1878,7 +2065,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>4.4000000000000004</v>
       </c>
@@ -1950,7 +2137,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>5.3</v>
       </c>
@@ -2018,7 +2205,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>5.6</v>
       </c>
@@ -2038,7 +2225,7 @@
       <c r="G25" s="6"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>6.1</v>
       </c>
@@ -2058,7 +2245,7 @@
       <c r="G26" s="6"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>6.2</v>
       </c>
@@ -2078,7 +2265,7 @@
       <c r="G27" s="6"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>6.3</v>
       </c>
@@ -2098,7 +2285,7 @@
       <c r="G28" s="6"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>6.4</v>
       </c>
@@ -2118,7 +2305,7 @@
       <c r="G29" s="6"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>6.5</v>
       </c>
@@ -2253,10 +2440,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB71BC0-4FED-421A-86C5-328962F1C9A8}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84:B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,7 +2453,7 @@
     <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>91</v>
       </c>
@@ -2276,15 +2463,18 @@
       <c r="C1" s="34" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="37" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="32">
         <v>1.2</v>
       </c>
       <c r="C2" s="31"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>206</v>
       </c>
@@ -2295,7 +2485,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>204</v>
       </c>
@@ -2306,7 +2496,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>202</v>
       </c>
@@ -2317,7 +2507,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>200</v>
       </c>
@@ -2328,7 +2518,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>198</v>
       </c>
@@ -2339,7 +2529,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>196</v>
       </c>
@@ -2350,7 +2540,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>194</v>
       </c>
@@ -2361,7 +2551,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>192</v>
       </c>
@@ -2372,7 +2562,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>190</v>
       </c>
@@ -2383,7 +2573,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>188</v>
       </c>
@@ -2394,7 +2584,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>186</v>
       </c>
@@ -2405,7 +2595,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>184</v>
       </c>
@@ -2416,7 +2606,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>182</v>
       </c>
@@ -2427,7 +2617,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>180</v>
       </c>
@@ -2889,7 +3079,321 @@
         <v>94</v>
       </c>
     </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="38" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="B61" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="C61" s="41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="40" t="s">
+        <v>219</v>
+      </c>
+      <c r="B62" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="C62" s="41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>210</v>
+      </c>
+      <c r="C63" s="41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>211</v>
+      </c>
+      <c r="C64" s="41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="B65" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="C65" s="43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="B66" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="C66" s="43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="B67" t="s">
+        <v>216</v>
+      </c>
+      <c r="C67" s="43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="B68" t="s">
+        <v>215</v>
+      </c>
+      <c r="C68" s="43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="39"/>
+      <c r="B69" s="40" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" s="43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="39"/>
+      <c r="B70" s="42" t="s">
+        <v>218</v>
+      </c>
+      <c r="C70" s="43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="13">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="C73" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74" t="s">
+        <v>228</v>
+      </c>
+      <c r="C74" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B75" t="s">
+        <v>229</v>
+      </c>
+      <c r="C75" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B76" t="s">
+        <v>230</v>
+      </c>
+      <c r="C76" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B77" t="s">
+        <v>231</v>
+      </c>
+      <c r="C77" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="B78" t="s">
+        <v>232</v>
+      </c>
+      <c r="C78" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="B79" t="s">
+        <v>233</v>
+      </c>
+      <c r="C79" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B80" t="s">
+        <v>238</v>
+      </c>
+      <c r="C80" s="44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B81" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="C81" s="44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="13" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="46" t="s">
+        <v>241</v>
+      </c>
+      <c r="B84" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="C84" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="B85" t="s">
+        <v>251</v>
+      </c>
+      <c r="C85" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="46" t="s">
+        <v>243</v>
+      </c>
+      <c r="B86" t="s">
+        <v>252</v>
+      </c>
+      <c r="C86" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="46" t="s">
+        <v>244</v>
+      </c>
+      <c r="B87" t="s">
+        <v>253</v>
+      </c>
+      <c r="C87" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="B88" t="s">
+        <v>254</v>
+      </c>
+      <c r="C88" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="46" t="s">
+        <v>246</v>
+      </c>
+      <c r="B89" t="s">
+        <v>255</v>
+      </c>
+      <c r="C89" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="46" t="s">
+        <v>247</v>
+      </c>
+      <c r="B90" t="s">
+        <v>256</v>
+      </c>
+      <c r="C90" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="B91" t="s">
+        <v>257</v>
+      </c>
+      <c r="C91" s="44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="B92" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="C92" s="44" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A3:C1048576">
     <cfRule type="expression" dxfId="4" priority="1">
       <formula>$C3="lead"</formula>

</xml_diff>